<commit_message>
these modifications fix all the bugs specifically issues #276 #262 #236 #193
</commit_message>
<xml_diff>
--- a/VocabolariControllati/licences/licences.xlsx
+++ b/VocabolariControllati/licences/licences.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11008"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Library/CloudStorage/Dropbox/OntoPiA/GitOntoPiA/daf-ontologie-vocabolari-controllati/VocabolariControllati/licences/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17A8C396-B627-F442-86A1-EE773BCB2286}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1680" yWindow="1680" windowWidth="23920" windowHeight="13860" tabRatio="500"/>
+    <workbookView xWindow="1680" yWindow="1680" windowWidth="23920" windowHeight="13860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="127">
   <si>
     <t>Tipo licenza livello 2</t>
   </si>
@@ -394,12 +400,18 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>B.1.17</t>
+  </si>
+  <si>
+    <t>Dichiarazioni di uso standard beni culturali (BCS)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -568,104 +580,112 @@
     </xf>
   </cellXfs>
   <cellStyles count="95">
-    <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento ipertestuale" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Collegamento visitato" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -990,14 +1010,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F41" sqref="F41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
@@ -1007,7 +1027,7 @@
     <col min="6" max="6" width="93.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
@@ -1027,7 +1047,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1047,7 +1067,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -1067,7 +1087,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1087,7 +1107,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1107,7 +1127,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -1127,7 +1147,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1147,7 +1167,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -1167,7 +1187,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -1187,7 +1207,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -1207,7 +1227,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -1227,7 +1247,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -1247,7 +1267,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -1267,7 +1287,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -1287,7 +1307,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -1307,7 +1327,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -1327,7 +1347,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -1347,7 +1367,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -1367,7 +1387,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1387,7 +1407,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -1407,7 +1427,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -1427,7 +1447,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -1447,7 +1467,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -1467,7 +1487,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -1487,7 +1507,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -1507,7 +1527,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1527,7 +1547,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1547,7 +1567,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1567,7 +1587,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>9</v>
       </c>
@@ -1587,7 +1607,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>9</v>
       </c>
@@ -1607,7 +1627,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>9</v>
       </c>
@@ -1627,7 +1647,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>9</v>
       </c>
@@ -1647,7 +1667,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="33" spans="1:6">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>9</v>
       </c>
@@ -1667,7 +1687,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:6">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>9</v>
       </c>
@@ -1687,7 +1707,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:6">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>9</v>
       </c>
@@ -1707,7 +1727,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:6">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>9</v>
       </c>
@@ -1727,7 +1747,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="37" spans="1:6">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>9</v>
       </c>
@@ -1747,7 +1767,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="1:6">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>9</v>
       </c>
@@ -1767,7 +1787,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="39" spans="1:6">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>9</v>
       </c>
@@ -1787,7 +1807,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:6">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>9</v>
       </c>
@@ -1807,7 +1827,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="41" spans="1:6">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>9</v>
       </c>
@@ -1827,27 +1847,27 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="1:6">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>9</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>102</v>
+      <c r="C42" s="4" t="s">
+        <v>65</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="F42" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>9</v>
       </c>
@@ -1861,13 +1881,13 @@
         <v>104</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F43" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>9</v>
       </c>
@@ -1881,13 +1901,13 @@
         <v>104</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F44" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>9</v>
       </c>
@@ -1901,13 +1921,13 @@
         <v>104</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F45" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>9</v>
       </c>
@@ -1921,13 +1941,13 @@
         <v>104</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F46" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>9</v>
       </c>
@@ -1941,13 +1961,13 @@
         <v>104</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F47" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>9</v>
       </c>
@@ -1961,13 +1981,13 @@
         <v>104</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F48" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>9</v>
       </c>
@@ -1981,13 +2001,13 @@
         <v>104</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F49" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>9</v>
       </c>
@@ -2001,29 +2021,49 @@
         <v>104</v>
       </c>
       <c r="E50" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F50" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>9</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E51" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="F50" t="s">
+      <c r="F51" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="51" spans="1:6">
-      <c r="A51" t="s">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
         <v>124</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B52" t="s">
         <v>82</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C52" t="s">
         <v>83</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D52" t="s">
         <v>82</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E52" t="s">
         <v>84</v>
       </c>
-      <c r="F51" t="s">
+      <c r="F52" t="s">
         <v>85</v>
       </c>
     </row>

</xml_diff>